<commit_message>
Added MLID properly with "empty_cols" in json
</commit_message>
<xml_diff>
--- a/Files/college_info/all_colleges/MLID/MLID_placements.xlsx
+++ b/Files/college_info/all_colleges/MLID/MLID_placements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mugdha\Desktop\python project\self\MLID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mugdha\Desktop\python project\github\python_project-dataset\Files\college_info\all_colleges\MLID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB57669A-CC8D-4362-B31D-462163576482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AB7E3A-5338-4220-9A54-849891E42936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Amazon</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Amadeus Labs</t>
   </si>
   <si>
-    <t>Infosys Limited</t>
-  </si>
-  <si>
     <t>HSBC Technology India</t>
   </si>
   <si>
@@ -68,12 +65,6 @@
     <t>Ert Technologies Pvt. Ltd.</t>
   </si>
   <si>
-    <t>Capgemini</t>
-  </si>
-  <si>
-    <t>Tata Consultancy Services</t>
-  </si>
-  <si>
     <t>Zensar Technologies</t>
   </si>
   <si>
@@ -83,18 +74,6 @@
     <t>Zemoso Technologies Pvt. Ltd.</t>
   </si>
   <si>
-    <t>Accenture</t>
-  </si>
-  <si>
-    <t>Virtusa Corporation</t>
-  </si>
-  <si>
-    <t>L&amp;T Infotech</t>
-  </si>
-  <si>
-    <t>Wipro Limited</t>
-  </si>
-  <si>
     <t>Infor India Pvt. Ltd.</t>
   </si>
   <si>
@@ -174,6 +153,51 @@
   </si>
   <si>
     <t>OFFERS</t>
+  </si>
+  <si>
+    <t>Accenture_6.5</t>
+  </si>
+  <si>
+    <t>Accenture_4.5</t>
+  </si>
+  <si>
+    <t>Capgemini_7.5</t>
+  </si>
+  <si>
+    <t>Capgemini_4</t>
+  </si>
+  <si>
+    <t>Infosys Limited_9.5</t>
+  </si>
+  <si>
+    <t>Infosys Limited_5</t>
+  </si>
+  <si>
+    <t>Infosys Limited_3.6</t>
+  </si>
+  <si>
+    <t>L&amp;T Infotech_6.5</t>
+  </si>
+  <si>
+    <t>L&amp;T Infotech_5</t>
+  </si>
+  <si>
+    <t>Tata Consultancy Services_7</t>
+  </si>
+  <si>
+    <t>Tata Consultancy Services_3.37</t>
+  </si>
+  <si>
+    <t>Virtusa Corporation_6.5</t>
+  </si>
+  <si>
+    <t>Virtusa Corporation_5.5</t>
+  </si>
+  <si>
+    <t>Wipro Limited_6.5</t>
+  </si>
+  <si>
+    <t>Wipro Limited_3.75</t>
   </si>
 </sst>
 </file>
@@ -553,7 +577,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,16 +588,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -623,7 +647,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="C5" s="3">
         <v>9.5</v>
@@ -637,7 +661,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="3">
         <v>9</v>
@@ -651,7 +675,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3">
         <v>8.92</v>
@@ -665,7 +689,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3">
         <v>8.17</v>
@@ -679,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3">
         <v>8.0299999999999994</v>
@@ -693,7 +717,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3">
         <v>8</v>
@@ -707,7 +731,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3">
         <v>8</v>
@@ -721,7 +745,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C12" s="3">
         <v>7.5</v>
@@ -735,7 +759,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="C13" s="3">
         <v>7</v>
@@ -748,28 +772,28 @@
       <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
+      <c r="B14" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C14" s="3">
         <v>7</v>
       </c>
-      <c r="D14" s="1">
-        <v>16</v>
+      <c r="D14" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="C15" s="3">
         <v>7</v>
       </c>
-      <c r="D15" s="2">
-        <v>9</v>
+      <c r="D15" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -777,7 +801,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3">
         <v>6.89</v>
@@ -791,7 +815,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3">
         <v>6.5</v>
@@ -805,7 +829,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C18" s="3">
         <v>6.5</v>
@@ -819,7 +843,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C19" s="3">
         <v>6.5</v>
@@ -828,18 +852,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C20" s="3">
         <v>6.5</v>
       </c>
       <c r="D20" s="2">
-        <v>74</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -847,13 +871,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="C21" s="3">
         <v>6.5</v>
       </c>
       <c r="D21" s="2">
-        <v>5</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,7 +885,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C22" s="3">
         <v>6</v>
@@ -870,18 +894,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>16</v>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C23" s="3">
         <v>5.5</v>
       </c>
       <c r="D23" s="1">
-        <v>107</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,7 +913,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C24" s="3">
         <v>5.5</v>
@@ -902,14 +926,14 @@
       <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>22</v>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="C25" s="3">
         <v>5.5</v>
       </c>
       <c r="D25" s="1">
-        <v>28</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -917,13 +941,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C26" s="3">
         <v>5</v>
       </c>
-      <c r="D26" s="1">
-        <v>16</v>
+      <c r="D26" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -931,41 +955,41 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C27" s="3">
         <v>5</v>
       </c>
-      <c r="D27" s="1">
-        <v>7</v>
+      <c r="D27" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>23</v>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C28" s="3">
         <v>5</v>
       </c>
-      <c r="D28" s="2">
-        <v>6</v>
+      <c r="D28" s="1">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>24</v>
+      <c r="B29" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C29" s="3">
         <v>5</v>
       </c>
       <c r="D29" s="1">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,13 +997,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C30" s="3">
         <v>5</v>
       </c>
-      <c r="D30" s="2">
-        <v>5</v>
+      <c r="D30" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,7 +1011,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C31" s="3">
         <v>5</v>
@@ -1001,7 +1025,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C32" s="3">
         <v>4.5</v>
@@ -1015,7 +1039,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C33" s="3">
         <v>4.5</v>
@@ -1029,7 +1053,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C34" s="3">
         <v>4.25</v>
@@ -1043,7 +1067,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C35" s="3">
         <v>4.2</v>
@@ -1057,7 +1081,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C36" s="3">
         <v>4.2</v>
@@ -1071,7 +1095,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="C37" s="3">
         <v>4</v>
@@ -1080,46 +1104,46 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>31</v>
+      <c r="B38" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C38" s="3">
         <v>4</v>
       </c>
-      <c r="D38" s="2">
-        <v>53</v>
+      <c r="D38" s="1">
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>38</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>32</v>
+      <c r="B39" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C39" s="3">
         <v>4</v>
       </c>
-      <c r="D39" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D39" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C40" s="3">
         <v>4</v>
       </c>
       <c r="D40" s="2">
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1127,7 +1151,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C41" s="3">
         <v>3.85</v>
@@ -1141,7 +1165,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C42" s="3">
         <v>3.75</v>
@@ -1155,13 +1179,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C43" s="3">
         <v>3.6</v>
       </c>
       <c r="D43" s="2">
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1169,41 +1193,41 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C44" s="3">
         <v>3.6</v>
       </c>
       <c r="D44" s="2">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>44</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>36</v>
+      <c r="B45" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C45" s="3">
         <v>3.5</v>
       </c>
-      <c r="D45" s="1">
-        <v>4</v>
+      <c r="D45" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>45</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>37</v>
+      <c r="B46" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C46" s="3">
         <v>3.5</v>
       </c>
-      <c r="D46" s="2">
-        <v>2</v>
+      <c r="D46" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1211,7 +1235,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="C47" s="3">
         <v>3.37</v>
@@ -1225,13 +1249,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C48" s="3">
         <v>3.25</v>
       </c>
       <c r="D48" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1239,7 +1263,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C49" s="3">
         <v>3.25</v>
@@ -1253,13 +1277,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C50" s="3">
         <v>3.25</v>
       </c>
       <c r="D50" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1267,7 +1291,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C51" s="3">
         <v>2.5</v>

</xml_diff>